<commit_message>
alustavaa ajankäyttöä, päivitetään maanantaina vastaamaan sprintin toteutusta
</commit_message>
<xml_diff>
--- a/Dokumentaatio/Tuntikirjanpitoa.xlsx
+++ b/Dokumentaatio/Tuntikirjanpitoa.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93e9b65c7ea9229f/Documents/koulu/tkt/ohtu/miniprojekti/ryhma16/Dokumentaatio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A059A80-B5ED-4DA3-ACFB-E7DBFE6682B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="8_{2A059A80-B5ED-4DA3-ACFB-E7DBFE6682B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4F151AE4-AD3A-4D6F-A5A1-EEA0B0CA83E3}"/>
   <bookViews>
-    <workbookView xWindow="7785" yWindow="900" windowWidth="19380" windowHeight="11385" xr2:uid="{93DED8CF-8FC2-4759-B3A9-EA8F0C6BF5A8}"/>
+    <workbookView xWindow="7365" yWindow="2175" windowWidth="19380" windowHeight="11385" activeTab="2" xr2:uid="{93DED8CF-8FC2-4759-B3A9-EA8F0C6BF5A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Ensimmäinen viikko tunnit" sheetId="1" r:id="rId1"/>
     <sheet name="Ensimmäinen viikko taskit" sheetId="2" r:id="rId2"/>
+    <sheet name="Toisen viikon tunnit" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="35">
   <si>
     <t>Atte</t>
   </si>
@@ -137,6 +138,9 @@
   </si>
   <si>
     <t>Tehty</t>
+  </si>
+  <si>
+    <t>Odotellaan infoa</t>
   </si>
 </sst>
 </file>
@@ -1718,6 +1722,986 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fi-FI"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Toisen viikon tuntikirjaus</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.21777077865266842"/>
+          <c:y val="4.6296296296296294E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-FI"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ensimmäinen viikko tunnit'!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Atte</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ensimmäinen viikko tunnit'!$C$2:$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>ma</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ti</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ke</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>to</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>pe</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>la</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>su</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Yhteensä</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ensimmäinen viikko tunnit'!$C$3:$J$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-67D9-458B-9B13-159B13055158}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ensimmäinen viikko tunnit'!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lauri</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ensimmäinen viikko tunnit'!$C$2:$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>ma</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ti</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ke</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>to</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>pe</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>la</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>su</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Yhteensä</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ensimmäinen viikko tunnit'!$C$4:$J$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-67D9-458B-9B13-159B13055158}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ensimmäinen viikko tunnit'!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dennis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ensimmäinen viikko tunnit'!$C$2:$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>ma</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ti</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ke</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>to</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>pe</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>la</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>su</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Yhteensä</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ensimmäinen viikko tunnit'!$C$5:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-67D9-458B-9B13-159B13055158}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ensimmäinen viikko tunnit'!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sonja</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ensimmäinen viikko tunnit'!$C$2:$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>ma</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ti</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ke</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>to</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>pe</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>la</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>su</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Yhteensä</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ensimmäinen viikko tunnit'!$C$6:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-67D9-458B-9B13-159B13055158}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ensimmäinen viikko tunnit'!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sami</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ensimmäinen viikko tunnit'!$C$2:$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>ma</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ti</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ke</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>to</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>pe</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>la</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>su</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Yhteensä</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ensimmäinen viikko tunnit'!$C$7:$J$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-67D9-458B-9B13-159B13055158}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ensimmäinen viikko tunnit'!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ossi</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ensimmäinen viikko tunnit'!$C$2:$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>ma</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ti</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ke</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>to</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>pe</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>la</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>su</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Yhteensä</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ensimmäinen viikko tunnit'!$C$8:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-67D9-458B-9B13-159B13055158}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="300"/>
+        <c:axId val="422867520"/>
+        <c:axId val="286061440"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="422867520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Ajanhetki</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-FI"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-FI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="286061440"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="286061440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Käytetty aika (h)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-FI"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-FI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="422867520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-FI"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-FI"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1798,6 +2782,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2763,6 +3787,509 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2861,6 +4388,49 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Kaavio 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA143E1E-D47E-4ED7-BAB1-636FEC09557A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3176,8 +4746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EB0CCA-0523-4C98-AB42-4C8E5DCF0E49}">
   <dimension ref="B2:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3733,4 +5303,231 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAFD0779-CDB8-401D-B376-7ADA8C60B602}">
+  <dimension ref="B2:J10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <f>SUM(C3:I3)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J8" si="0">SUM(C4:I4)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>